<commit_message>
Updated the data model documentation with the details of the citation import tables.
</commit_message>
<xml_diff>
--- a/Documentation/DataModel/BHLDataDictionary.xlsx
+++ b/Documentation/DataModel/BHLDataDictionary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6053" uniqueCount="1076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6672" uniqueCount="1145">
   <si>
     <t>DATA_TYPE</t>
   </si>
@@ -3274,6 +3274,213 @@
   </si>
   <si>
     <t>Counts of various BHL entities (ex. Titles, Items).  Accumulating these counts can be time-consuming, so the values contained in this table are used to display counts when performance is important and real-time accuracy is not crucial.</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>ImportFile</t>
+  </si>
+  <si>
+    <t>ImportFileID</t>
+  </si>
+  <si>
+    <t>ImportFileStatusID</t>
+  </si>
+  <si>
+    <t>ImportFileName</t>
+  </si>
+  <si>
+    <t>ImportFileStatus</t>
+  </si>
+  <si>
+    <t>ImportRecord</t>
+  </si>
+  <si>
+    <t>ImportRecordID</t>
+  </si>
+  <si>
+    <t>ImportRecordStatusID</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>JournalTitle</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>StartPage</t>
+  </si>
+  <si>
+    <t>EndPage</t>
+  </si>
+  <si>
+    <t>LCCN</t>
+  </si>
+  <si>
+    <t>ImportRecordCreator</t>
+  </si>
+  <si>
+    <t>ImportRecordCreatorID</t>
+  </si>
+  <si>
+    <t>ImportRecordErrorLog</t>
+  </si>
+  <si>
+    <t>ImportRecordErrorLogID</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>ImportRecordKeyword</t>
+  </si>
+  <si>
+    <t>ImportRecordKeywordID</t>
+  </si>
+  <si>
+    <t>ImportRecordStatus</t>
+  </si>
+  <si>
+    <t>Identifier of the file from which this record originated.</t>
+  </si>
+  <si>
+    <t>Identifier of the record status.</t>
+  </si>
+  <si>
+    <t>Identifier of the imported record.</t>
+  </si>
+  <si>
+    <t>The keyword</t>
+  </si>
+  <si>
+    <t>Errors encountered when processing imported citations.</t>
+  </si>
+  <si>
+    <t>Keywords/subjects that apply to imported citations.</t>
+  </si>
+  <si>
+    <t>Authors associated with imported citations.</t>
+  </si>
+  <si>
+    <t>Date and time of the error.</t>
+  </si>
+  <si>
+    <t>Details of the error.</t>
+  </si>
+  <si>
+    <t>Statuses of imported citations (ex. New, Imported, Rejected, Error).</t>
+  </si>
+  <si>
+    <t>Processing statuses of files containing citations (ex. Loading , New, Imported, Rejected).</t>
+  </si>
+  <si>
+    <t>Files containing citations to be imported into BHL.</t>
+  </si>
+  <si>
+    <t>Name of the file.</t>
+  </si>
+  <si>
+    <t>A citation to be imported into BHL.</t>
+  </si>
+  <si>
+    <t>The full name of the author.  This might be the combined first and last names of a person, the name of a corporation, or the name of a conference/meeting.</t>
+  </si>
+  <si>
+    <t>Last name of the author.</t>
+  </si>
+  <si>
+    <t>First name of the author.</t>
+  </si>
+  <si>
+    <t>Identifies the type of the author. (ex. Person, corporation)</t>
+  </si>
+  <si>
+    <t>Genre of the cited work.</t>
+  </si>
+  <si>
+    <t>Title of the cited work.</t>
+  </si>
+  <si>
+    <t>Translated title of the cited work.</t>
+  </si>
+  <si>
+    <t>Title of the container of the cited work.  For example, the container of an article would be the journal in which the article appears.</t>
+  </si>
+  <si>
+    <t>Complete publication details (Name, Place, Date) for the cited work.</t>
+  </si>
+  <si>
+    <t>Publisher of the cited work.</t>
+  </si>
+  <si>
+    <t>Place of publication of the cited work.</t>
+  </si>
+  <si>
+    <t>Year of the cited work.</t>
+  </si>
+  <si>
+    <t>End year of the cited work (for example, if a journal is cited)</t>
+  </si>
+  <si>
+    <t>Start year of the cited work (for example, if a journal is cited)</t>
+  </si>
+  <si>
+    <t>The range of pages in the container on which the cited work appears.</t>
+  </si>
+  <si>
+    <t>First page number in the container on which the cited work appears.</t>
+  </si>
+  <si>
+    <t>Last page number in the container on which the cited work appears.</t>
+  </si>
+  <si>
+    <t>Language of the cited work.</t>
+  </si>
+  <si>
+    <t>URL of a location external to BHL at which the cited work is located</t>
+  </si>
+  <si>
+    <t>URL for downloading the cited work.</t>
+  </si>
+  <si>
+    <t>ISSN of the cited work (or the work's container)</t>
+  </si>
+  <si>
+    <t>ISBN of the cited work (or the work's container)</t>
+  </si>
+  <si>
+    <t>OCLC # of the cited work (or the work's container)</t>
+  </si>
+  <si>
+    <t>LCCN of the cited work (or the work's container)</t>
+  </si>
+  <si>
+    <t>DOI of the cited work (or the work's container).</t>
+  </si>
+  <si>
+    <t>Rights statement of the cited work.</t>
+  </si>
+  <si>
+    <t>Copyright status of the cited work.</t>
+  </si>
+  <si>
+    <t>Name of the license that applies to this cited work's content.</t>
+  </si>
+  <si>
+    <t>URL to the license (ex. Creative Commons) that applies to the cited work's content.</t>
+  </si>
+  <si>
+    <t>Due diligence statement of the cited work.</t>
+  </si>
+  <si>
+    <t>Summary or abstract of the cited work.</t>
+  </si>
+  <si>
+    <t>General notes about the cited work.</t>
   </si>
 </sst>
 </file>
@@ -3667,11 +3874,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1044"/>
+  <dimension ref="A1:I1146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A306" sqref="A306"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -3679,8 +3886,7 @@
     <col min="1" max="1" width="8.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="4" customWidth="1"/>
     <col min="7" max="7" width="7" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
@@ -26443,7 +26649,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="1035" spans="1:9" ht="409.6">
+    <row r="1035" spans="1:9">
       <c r="A1035" s="4" t="s">
         <v>111</v>
       </c>
@@ -26521,11 +26727,11 @@
         <v>774</v>
       </c>
     </row>
-    <row r="1038" spans="1:9" s="9" customFormat="1" ht="409.6">
+    <row r="1038" spans="1:9" s="9" customFormat="1">
       <c r="G1038" s="10"/>
       <c r="I1038" s="11"/>
     </row>
-    <row r="1039" spans="1:9" ht="409.6">
+    <row r="1039" spans="1:9">
       <c r="A1039" s="4" t="s">
         <v>111</v>
       </c>
@@ -26562,7 +26768,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="1041" spans="1:9" ht="409.6">
+    <row r="1041" spans="1:9">
       <c r="A1041" s="4" t="s">
         <v>111</v>
       </c>
@@ -26585,7 +26791,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="1042" spans="1:9" ht="409.6">
+    <row r="1042" spans="1:9">
       <c r="A1042" s="4" t="s">
         <v>111</v>
       </c>
@@ -26652,6 +26858,2609 @@
       </c>
       <c r="I1044" s="6" t="s">
         <v>830</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:9" s="9" customFormat="1">
+      <c r="G1045" s="10"/>
+      <c r="I1045" s="11"/>
+    </row>
+    <row r="1046" spans="1:9">
+      <c r="A1046" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1046" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="I1046" s="6" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:9">
+      <c r="A1047" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1047" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C1047" s="4" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D1047" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1047" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1047" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1047" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1047" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:9">
+      <c r="A1048" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1048" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C1048" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D1048" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1048" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1048" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1048" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1048" s="6" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:9">
+      <c r="A1049" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1049" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C1049" s="4" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D1049" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1049" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1049" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1049" s="4">
+        <v>200</v>
+      </c>
+      <c r="I1049" s="6" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:9">
+      <c r="A1050" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1050" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C1050" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D1050" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1050" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1050" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1050" s="4">
+        <v>10</v>
+      </c>
+      <c r="I1050" s="6" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:9">
+      <c r="A1051" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1051" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C1051" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1051" s="4">
+        <v>5</v>
+      </c>
+      <c r="E1051" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1051" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1051" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1051" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1051" s="6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:9">
+      <c r="A1052" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1052" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C1052" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1052" s="4">
+        <v>6</v>
+      </c>
+      <c r="E1052" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1052" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1052" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1052" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1052" s="6" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:9">
+      <c r="A1053" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1053" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C1053" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1053" s="4">
+        <v>7</v>
+      </c>
+      <c r="E1053" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1053" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1053" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1053" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1053" s="6" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:9" ht="22.5">
+      <c r="A1054" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1054" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C1054" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1054" s="4">
+        <v>8</v>
+      </c>
+      <c r="E1054" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1054" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1054" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1054" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1054" s="6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:9" s="9" customFormat="1">
+      <c r="G1055" s="10"/>
+      <c r="I1055" s="11"/>
+    </row>
+    <row r="1056" spans="1:9" ht="22.5">
+      <c r="A1056" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1056" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="I1056" s="6" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:9">
+      <c r="A1057" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1057" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C1057" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D1057" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1057" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1057" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1057" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1057" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:9">
+      <c r="A1058" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1058" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C1058" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D1058" s="4">
+        <v>2</v>
+      </c>
+      <c r="E1058" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1058" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1058" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1058" s="4">
+        <v>50</v>
+      </c>
+      <c r="I1058" s="6" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:9">
+      <c r="A1059" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1059" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C1059" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1059" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1059" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1059" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1059" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1059" s="4">
+        <v>500</v>
+      </c>
+      <c r="I1059" s="6" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:9">
+      <c r="A1060" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1060" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C1060" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1060" s="4">
+        <v>4</v>
+      </c>
+      <c r="E1060" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1060" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1060" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1060" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1060" s="6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:9">
+      <c r="A1061" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1061" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C1061" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1061" s="4">
+        <v>5</v>
+      </c>
+      <c r="E1061" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1061" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1061" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1061" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1061" s="6" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:9">
+      <c r="A1062" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1062" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C1062" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1062" s="4">
+        <v>6</v>
+      </c>
+      <c r="E1062" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1062" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1062" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1062" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1062" s="6" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:9" ht="22.5">
+      <c r="A1063" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1063" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C1063" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1063" s="4">
+        <v>7</v>
+      </c>
+      <c r="E1063" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1063" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1063" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1063" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1063" s="6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:9" s="9" customFormat="1">
+      <c r="G1064" s="10"/>
+      <c r="I1064" s="11"/>
+    </row>
+    <row r="1065" spans="1:9">
+      <c r="A1065" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1065" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="I1065" s="6" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:9">
+      <c r="A1066" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1066" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1066" s="4" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D1066" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1066" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1066" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1066" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1066" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:9" ht="22.5">
+      <c r="A1067" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1067" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1067" s="4" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D1067" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1067" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1067" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1067" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1067" s="6" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:9">
+      <c r="A1068" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1068" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1068" s="4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D1068" s="4">
+        <v>3</v>
+      </c>
+      <c r="F1068" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1068" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1068" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1068" s="6" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:9">
+      <c r="A1069" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1069" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1069" s="4" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D1069" s="4">
+        <v>4</v>
+      </c>
+      <c r="E1069" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1069" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1069" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1069" s="4">
+        <v>50</v>
+      </c>
+      <c r="I1069" s="6" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:9">
+      <c r="A1070" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1070" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1070" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1070" s="4">
+        <v>5</v>
+      </c>
+      <c r="E1070" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1070" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1070" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1070" s="4">
+        <v>2000</v>
+      </c>
+      <c r="I1070" s="6" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:9">
+      <c r="A1071" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1071" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1071" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="D1071" s="4">
+        <v>6</v>
+      </c>
+      <c r="E1071" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1071" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1071" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1071" s="4">
+        <v>2000</v>
+      </c>
+      <c r="I1071" s="6" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:9" ht="33.75">
+      <c r="A1072" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1072" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1072" s="4" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D1072" s="4">
+        <v>7</v>
+      </c>
+      <c r="E1072" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1072" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1072" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1072" s="4">
+        <v>2000</v>
+      </c>
+      <c r="I1072" s="6" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:9">
+      <c r="A1073" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1073" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1073" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1073" s="4">
+        <v>8</v>
+      </c>
+      <c r="E1073" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1073" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1073" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1073" s="4">
+        <v>100</v>
+      </c>
+      <c r="I1073" s="6" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:9">
+      <c r="A1074" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1074" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1074" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1074" s="4">
+        <v>9</v>
+      </c>
+      <c r="E1074" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1074" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1074" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1074" s="4">
+        <v>100</v>
+      </c>
+      <c r="I1074" s="6" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:9">
+      <c r="A1075" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1075" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1075" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D1075" s="4">
+        <v>10</v>
+      </c>
+      <c r="E1075" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1075" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1075" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1075" s="4">
+        <v>100</v>
+      </c>
+      <c r="I1075" s="6" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:9">
+      <c r="A1076" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1076" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1076" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1076" s="4">
+        <v>11</v>
+      </c>
+      <c r="E1076" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1076" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1076" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1076" s="4">
+        <v>400</v>
+      </c>
+      <c r="I1076" s="6" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:9" ht="22.5">
+      <c r="A1077" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1077" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1077" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1077" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1077" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1077" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1077" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1077" s="4">
+        <v>400</v>
+      </c>
+      <c r="I1077" s="6" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:9">
+      <c r="A1078" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1078" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1078" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="D1078" s="4">
+        <v>13</v>
+      </c>
+      <c r="E1078" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1078" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1078" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1078" s="4">
+        <v>250</v>
+      </c>
+      <c r="I1078" s="6" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:9">
+      <c r="A1079" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1079" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1079" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D1079" s="4">
+        <v>14</v>
+      </c>
+      <c r="E1079" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1079" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1079" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1079" s="4">
+        <v>150</v>
+      </c>
+      <c r="I1079" s="6" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:9">
+      <c r="A1080" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1080" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1080" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1080" s="4">
+        <v>15</v>
+      </c>
+      <c r="E1080" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1080" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1080" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1080" s="4">
+        <v>20</v>
+      </c>
+      <c r="I1080" s="6" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:9" ht="22.5">
+      <c r="A1081" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1081" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1081" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="D1081" s="4">
+        <v>16</v>
+      </c>
+      <c r="F1081" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1081" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1081" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1081" s="6" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:9" ht="22.5">
+      <c r="A1082" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1082" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1082" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="D1082" s="4">
+        <v>17</v>
+      </c>
+      <c r="F1082" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1082" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1082" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1082" s="6" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:9">
+      <c r="A1083" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1083" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1083" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1083" s="4">
+        <v>18</v>
+      </c>
+      <c r="F1083" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1083" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1083" s="4">
+        <v>30</v>
+      </c>
+      <c r="I1083" s="6" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:9">
+      <c r="A1084" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1084" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1084" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="D1084" s="4">
+        <v>19</v>
+      </c>
+      <c r="E1084" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1084" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1084" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1084" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I1084" s="6" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:9">
+      <c r="A1085" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1085" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1085" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="D1085" s="4">
+        <v>20</v>
+      </c>
+      <c r="E1085" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1085" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1085" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1085" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I1085" s="6" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:9">
+      <c r="A1086" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1086" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1086" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1086" s="4">
+        <v>21</v>
+      </c>
+      <c r="E1086" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1086" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1086" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1086" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I1086" s="6" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:9">
+      <c r="A1087" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1087" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1087" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1087" s="4">
+        <v>22</v>
+      </c>
+      <c r="E1087" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1087" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1087" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1087" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I1087" s="6" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:9">
+      <c r="A1088" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1088" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1088" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1088" s="4">
+        <v>23</v>
+      </c>
+      <c r="E1088" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1088" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1088" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1088" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I1088" s="6" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:9" ht="22.5">
+      <c r="A1089" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1089" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1089" s="4" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D1089" s="4">
+        <v>24</v>
+      </c>
+      <c r="E1089" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1089" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1089" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1089" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I1089" s="6" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:9" ht="22.5">
+      <c r="A1090" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1090" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1090" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D1090" s="4">
+        <v>25</v>
+      </c>
+      <c r="E1090" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1090" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1090" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1090" s="4">
+        <v>200</v>
+      </c>
+      <c r="I1090" s="6" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:9" ht="22.5">
+      <c r="A1091" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1091" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1091" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="D1091" s="4">
+        <v>26</v>
+      </c>
+      <c r="E1091" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1091" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1091" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1091" s="4">
+        <v>50</v>
+      </c>
+      <c r="I1091" s="6" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:9" ht="22.5">
+      <c r="A1092" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1092" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1092" s="4" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D1092" s="4">
+        <v>27</v>
+      </c>
+      <c r="E1092" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1092" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1092" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1092" s="4">
+        <v>20</v>
+      </c>
+      <c r="I1092" s="6" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:9" ht="22.5">
+      <c r="A1093" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1093" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1093" s="4" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D1093" s="4">
+        <v>28</v>
+      </c>
+      <c r="E1093" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1093" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1093" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1093" s="4">
+        <v>20</v>
+      </c>
+      <c r="I1093" s="6" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:9" ht="22.5">
+      <c r="A1094" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1094" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1094" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="D1094" s="4">
+        <v>29</v>
+      </c>
+      <c r="E1094" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1094" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1094" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1094" s="4">
+        <v>200</v>
+      </c>
+      <c r="I1094" s="6" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:9">
+      <c r="A1095" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1095" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1095" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1095" s="4">
+        <v>30</v>
+      </c>
+      <c r="E1095" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1095" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1095" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1095" s="4">
+        <v>200</v>
+      </c>
+      <c r="I1095" s="6" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:9">
+      <c r="A1096" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1096" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1096" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1096" s="4">
+        <v>31</v>
+      </c>
+      <c r="E1096" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1096" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1096" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1096" s="4">
+        <v>125</v>
+      </c>
+      <c r="I1096" s="6" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:9">
+      <c r="A1097" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1097" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1097" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D1097" s="4">
+        <v>32</v>
+      </c>
+      <c r="E1097" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1097" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1097" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1097" s="4">
+        <v>125</v>
+      </c>
+      <c r="I1097" s="6" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:9">
+      <c r="A1098" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1098" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1098" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1098" s="4">
+        <v>33</v>
+      </c>
+      <c r="E1098" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1098" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1098" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1098" s="4">
+        <v>125</v>
+      </c>
+      <c r="I1098" s="6" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:9" ht="22.5">
+      <c r="A1099" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1099" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1099" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D1099" s="4">
+        <v>34</v>
+      </c>
+      <c r="E1099" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1099" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1099" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1099" s="4">
+        <v>125</v>
+      </c>
+      <c r="I1099" s="6" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:9">
+      <c r="A1100" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1100" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1100" s="4" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D1100" s="4">
+        <v>35</v>
+      </c>
+      <c r="E1100" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1100" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1100" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1100" s="4">
+        <v>125</v>
+      </c>
+      <c r="I1100" s="6" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:9">
+      <c r="A1101" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1101" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1101" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1101" s="4">
+        <v>36</v>
+      </c>
+      <c r="E1101" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1101" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1101" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1101" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1101" s="6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:9">
+      <c r="A1102" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1102" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1102" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1102" s="4">
+        <v>37</v>
+      </c>
+      <c r="E1102" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1102" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1102" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1102" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1102" s="6" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:9">
+      <c r="A1103" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1103" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1103" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1103" s="4">
+        <v>38</v>
+      </c>
+      <c r="E1103" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1103" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1103" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1103" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1103" s="6" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:9" ht="22.5">
+      <c r="A1104" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1104" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C1104" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1104" s="4">
+        <v>39</v>
+      </c>
+      <c r="E1104" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1104" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1104" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1104" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1104" s="6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:9" s="9" customFormat="1">
+      <c r="G1105" s="10"/>
+      <c r="I1105" s="11"/>
+    </row>
+    <row r="1106" spans="1:9">
+      <c r="A1106" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1106" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="I1106" s="6" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:9">
+      <c r="A1107" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1107" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1107" s="4" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D1107" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1107" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1107" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1107" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1107" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:9">
+      <c r="A1108" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1108" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1108" s="4" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D1108" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1108" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1108" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1108" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1108" s="6" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:9" ht="45">
+      <c r="A1109" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1109" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1109" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1109" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1109" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1109" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1109" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1109" s="4">
+        <v>300</v>
+      </c>
+      <c r="I1109" s="6" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:9">
+      <c r="A1110" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1110" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1110" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1110" s="4">
+        <v>4</v>
+      </c>
+      <c r="E1110" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1110" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1110" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1110" s="4">
+        <v>150</v>
+      </c>
+      <c r="I1110" s="6" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:9">
+      <c r="A1111" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1111" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1111" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1111" s="4">
+        <v>5</v>
+      </c>
+      <c r="E1111" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1111" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1111" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1111" s="4">
+        <v>150</v>
+      </c>
+      <c r="I1111" s="6" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:9" ht="33.75">
+      <c r="A1112" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1112" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1112" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="D1112" s="4">
+        <v>6</v>
+      </c>
+      <c r="E1112" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1112" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1112" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1112" s="4">
+        <v>25</v>
+      </c>
+      <c r="I1112" s="6" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:9" ht="33.75">
+      <c r="A1113" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1113" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1113" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="D1113" s="4">
+        <v>7</v>
+      </c>
+      <c r="E1113" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1113" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1113" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1113" s="4">
+        <v>25</v>
+      </c>
+      <c r="I1113" s="6" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:9" ht="22.5">
+      <c r="A1114" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1114" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1114" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1114" s="4">
+        <v>8</v>
+      </c>
+      <c r="E1114" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1114" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1114" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1114" s="4">
+        <v>50</v>
+      </c>
+      <c r="I1114" s="6" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:9">
+      <c r="A1115" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1115" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1115" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1115" s="4">
+        <v>9</v>
+      </c>
+      <c r="E1115" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1115" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1115" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1115" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1115" s="6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:9">
+      <c r="A1116" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1116" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1116" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1116" s="4">
+        <v>10</v>
+      </c>
+      <c r="E1116" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1116" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1116" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1116" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1116" s="6" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:9">
+      <c r="A1117" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1117" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1117" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1117" s="4">
+        <v>11</v>
+      </c>
+      <c r="E1117" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1117" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1117" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1117" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1117" s="6" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:9" ht="22.5">
+      <c r="A1118" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1118" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C1118" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1118" s="4">
+        <v>12</v>
+      </c>
+      <c r="E1118" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1118" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1118" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1118" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1118" s="6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:9" s="9" customFormat="1">
+      <c r="G1119" s="10"/>
+      <c r="I1119" s="11"/>
+    </row>
+    <row r="1120" spans="1:9" ht="22.5">
+      <c r="A1120" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1120" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="I1120" s="6" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:9">
+      <c r="A1121" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1121" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C1121" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D1121" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1121" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1121" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1121" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1121" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:9">
+      <c r="A1122" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1122" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C1122" s="4" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D1122" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1122" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1122" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1122" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1122" s="6" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:9">
+      <c r="A1123" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1123" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C1123" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D1123" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1123" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1123" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1123" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1123" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1123" s="6" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:9">
+      <c r="A1124" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1124" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C1124" s="4" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D1124" s="4">
+        <v>4</v>
+      </c>
+      <c r="E1124" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1124" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1124" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1124" s="4">
+        <v>-1</v>
+      </c>
+      <c r="I1124" s="6" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:9">
+      <c r="A1125" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1125" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C1125" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1125" s="4">
+        <v>5</v>
+      </c>
+      <c r="E1125" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1125" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1125" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1125" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1125" s="6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:9">
+      <c r="A1126" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1126" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C1126" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1126" s="4">
+        <v>6</v>
+      </c>
+      <c r="E1126" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1126" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1126" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1126" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1126" s="6" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:9">
+      <c r="A1127" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1127" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C1127" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1127" s="4">
+        <v>7</v>
+      </c>
+      <c r="E1127" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1127" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1127" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1127" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1127" s="6" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:9" ht="22.5">
+      <c r="A1128" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1128" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C1128" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1128" s="4">
+        <v>8</v>
+      </c>
+      <c r="E1128" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1128" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1128" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1128" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1128" s="6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:9" s="9" customFormat="1">
+      <c r="G1129" s="10"/>
+      <c r="I1129" s="11"/>
+    </row>
+    <row r="1130" spans="1:9" ht="22.5">
+      <c r="A1130" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1130" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I1130" s="6" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:9">
+      <c r="A1131" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1131" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C1131" s="4" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D1131" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1131" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1131" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1131" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1131" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:9">
+      <c r="A1132" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1132" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C1132" s="4" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D1132" s="4">
+        <v>2</v>
+      </c>
+      <c r="F1132" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1132" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1132" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1132" s="6" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:9">
+      <c r="A1133" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1133" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C1133" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1133" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1133" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1133" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1133" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1133" s="4">
+        <v>50</v>
+      </c>
+      <c r="I1133" s="6" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:9">
+      <c r="A1134" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1134" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C1134" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1134" s="4">
+        <v>4</v>
+      </c>
+      <c r="E1134" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1134" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1134" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1134" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1134" s="6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:9">
+      <c r="A1135" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1135" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C1135" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1135" s="4">
+        <v>5</v>
+      </c>
+      <c r="E1135" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1135" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1135" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1135" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1135" s="6" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:9">
+      <c r="A1136" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1136" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C1136" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1136" s="4">
+        <v>6</v>
+      </c>
+      <c r="E1136" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1136" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1136" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1136" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1136" s="6" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:9" ht="22.5">
+      <c r="A1137" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1137" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C1137" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1137" s="4">
+        <v>7</v>
+      </c>
+      <c r="E1137" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1137" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1137" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1137" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1137" s="6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:9" s="9" customFormat="1">
+      <c r="G1138" s="10"/>
+      <c r="I1138" s="11"/>
+    </row>
+    <row r="1139" spans="1:9" ht="22.5">
+      <c r="A1139" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1139" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I1139" s="6" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:9">
+      <c r="A1140" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1140" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C1140" s="4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D1140" s="4">
+        <v>1</v>
+      </c>
+      <c r="F1140" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1140" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1140" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1140" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:9">
+      <c r="A1141" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1141" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C1141" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D1141" s="4">
+        <v>2</v>
+      </c>
+      <c r="E1141" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1141" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1141" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1141" s="4">
+        <v>50</v>
+      </c>
+      <c r="I1141" s="6" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:9">
+      <c r="A1142" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1142" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C1142" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1142" s="4">
+        <v>3</v>
+      </c>
+      <c r="E1142" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1142" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1142" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1142" s="4">
+        <v>500</v>
+      </c>
+      <c r="I1142" s="6" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:9">
+      <c r="A1143" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1143" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C1143" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1143" s="4">
+        <v>4</v>
+      </c>
+      <c r="E1143" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1143" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1143" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1143" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1143" s="6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:9">
+      <c r="A1144" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1144" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C1144" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1144" s="4">
+        <v>5</v>
+      </c>
+      <c r="E1144" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1144" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1144" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1144" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1144" s="6" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:9">
+      <c r="A1145" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1145" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C1145" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1145" s="4">
+        <v>6</v>
+      </c>
+      <c r="E1145" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1145" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1145" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1145" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1145" s="6" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:9" ht="22.5">
+      <c r="A1146" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1146" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C1146" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1146" s="4">
+        <v>7</v>
+      </c>
+      <c r="E1146" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1146" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1146" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1146" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1146" s="6" t="s">
+        <v>546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Public UI, API, and Export changes for Virtual Issues
</commit_message>
<xml_diff>
--- a/Documentation/DataModel/BHLDataDictionary.xlsx
+++ b/Documentation/DataModel/BHLDataDictionary.xlsx
@@ -4639,8 +4639,8 @@
   <dimension ref="A1:O1426"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1006" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1017" sqref="A1017"/>
+      <pane ySplit="1" topLeftCell="A967" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C978" sqref="C978"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -11263,7 +11263,7 @@
         <v>11</v>
       </c>
       <c r="G304" s="4">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="H304" s="4"/>
       <c r="I304" s="6" t="s">
@@ -26247,7 +26247,7 @@
         <v>11</v>
       </c>
       <c r="G978" s="4">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="H978" s="4"/>
       <c r="I978" s="6" t="s">

</xml_diff>

<commit_message>
Expanded Barcode-Identifier fields in import databases to 200 characters
</commit_message>
<xml_diff>
--- a/Documentation/DataModel/BHLDataDictionary.xlsx
+++ b/Documentation/DataModel/BHLDataDictionary.xlsx
@@ -4639,8 +4639,8 @@
   <dimension ref="A1:O1426"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1006" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1017" sqref="A1017"/>
+      <pane ySplit="1" topLeftCell="A967" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C978" sqref="C978"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -11263,7 +11263,7 @@
         <v>11</v>
       </c>
       <c r="G304" s="4">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="H304" s="4"/>
       <c r="I304" s="6" t="s">
@@ -26247,7 +26247,7 @@
         <v>11</v>
       </c>
       <c r="G978" s="4">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="H978" s="4"/>
       <c r="I978" s="6" t="s">

</xml_diff>